<commit_message>
created mermaid gantt chart
</commit_message>
<xml_diff>
--- a/Files/Gantt.xlsx
+++ b/Files/Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="499" documentId="8_{A108D8B6-617D-4728-A2E3-C3A56B5C1CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B31A3D95-4BBA-4E1F-82A1-08352205200B}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="8_{A108D8B6-617D-4728-A2E3-C3A56B5C1CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E215A2C9-8D05-4AC7-8610-C05CCD2ACC9D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2895" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1533,8 +1533,8 @@
   </sheetPr>
   <dimension ref="B1:BO99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1965,7 +1965,9 @@
       <c r="E7" s="58">
         <v>10</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="58">
+        <v>1</v>
+      </c>
       <c r="G7" s="22"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -8289,7 +8291,7 @@
   <dimension ref="B1:BO24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -10101,8 +10103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808C5D50-470B-44ED-B21F-9AB1AFD96A4E}">
   <dimension ref="B1:BO99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>

</xml_diff>